<commit_message>
Update notebooks and reports
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada-Coimbra-cargos_tarefas.datas.xlsx
+++ b/notebooks/jesuita-entrada-Coimbra-cargos_tarefas.datas.xlsx
@@ -457,436 +457,436 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>André Palmeiro</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Analista das missões da China e do Japão</t>
+          <t>Visitador das províncias de Goa e do Malabar</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1583</t>
+          <t>1621</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1596</t>
+          <t>1626</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gaspar Ferreira</t>
+          <t>André Palmeiro</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mestre dos Noviços</t>
+          <t>Visitador das províncias do Malabar</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1607</t>
+          <t>1618</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1607</t>
+          <t>1621</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>André Palmeiro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Monitor de Alessandro Valignano</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1579</t>
+          <t>1626</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1579</t>
+          <t>1635</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>José Montanha</t>
+          <t>António Gomes</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Procurador</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>1748</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>1751</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Manuel Gaspar</t>
+          <t>António da Silva</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Procurador da China e do Japão</t>
+          <t>Reitor de Nanquim</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1603</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1603</t>
+          <t>1699</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>António da Silva</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Procurador da Província do Japão em Macau</t>
+          <t>Socius do bispo de Nanquim</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1700</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>António da Silva</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1711</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1714</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Provincial de Goa</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1631</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1634</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Procurador do Japão</t>
+          <t>Superior de Agra</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1717</t>
+          <t>1624</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1717</t>
+          <t>1624</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Provincial da Etiópia</t>
+          <t>Visitador de Agra</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1555</t>
+          <t>1624</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1555</t>
+          <t>1624</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Provincial das Índias Orientais</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1559</t>
+          <t>1634</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1572</t>
+          <t>1634</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Pedro Martins</t>
+          <t>António de Gouveia</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Provincial das Índias Orientais</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1669</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1672</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>António de Gouveia</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Provincial de Goa</t>
+          <t>Visitador</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1666</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1634</t>
+          <t>1666</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Francisco Pacheco</t>
+          <t>Belchior Nunes Barreto</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Vice-provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1621</t>
+          <t>1553</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1625</t>
+          <t>1553</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Belchior Nunes Barreto</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Vice-provincial de Cochim</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1646</t>
+          <t>1565</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1649</t>
+          <t>1565</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Belchior Nunes Barreto</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Visitador da Província da Índia</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1566</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1661</t>
+          <t>1566</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Cristóvão da Costa</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Superior de Macau</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1702</t>
+          <t>1576</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1718</t>
+          <t>1576</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Estanislau Machado</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -896,18 +896,18 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1717</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1710</t>
+          <t>1718</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Superior da missão do Tonquim</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -932,107 +932,107 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>José Montanha</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Superior das seis residências do Norte</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1749</t>
+          <t>1641</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1752</t>
+          <t>1650</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Mateus de Couros</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Provincial do Japão e da China</t>
+          <t>Vice-provincial da China do Norte</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1617</t>
+          <t>1635</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1632</t>
+          <t>1641</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pedro Martins</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Reitor de Goa</t>
+          <t>Vice-provincial da China do Sul</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1646</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1646</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>António da Silva</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Reitor de Nanquim</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1041,27 +1041,27 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Reitor do Colégio de Macau</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1608</t>
+          <t>1621</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1611</t>
+          <t>1625</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Francisco Pacheco</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1071,222 +1071,222 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1608</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1611</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Francisco Pacheco</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Reitor do colégio de Macau</t>
+          <t>Superior da missão da China</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1623</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1623</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Manuel de Sá</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Socius de Francesco Maria Spinola</t>
+          <t>Procurador do Japão</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1717</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1717</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>António da Silva</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Socius do bispo de Nanquim</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>1705</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>1710</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Leonardo Teixeira</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Superior da China</t>
+          <t>Vice-visitador do Japão</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1559</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1572</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>João da Rocha</t>
+          <t>Francisco Pérez</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Superior da missão da China</t>
+          <t>Superior das Índias</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1622</t>
+          <t>1552</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1622</t>
+          <t>1552</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Francisco Pacheco</t>
+          <t>Francisco Pérez</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Superior da missão da China</t>
+          <t>Superior de Macau</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1565</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1565</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Gaspar Ferreira</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Superior da missão do Tonquim</t>
+          <t>Mestre dos Noviços</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1607</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1607</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Estanislau Machado</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1296,247 +1296,247 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1717</t>
+          <t>1631</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1718</t>
+          <t>1631</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Superior da residência de Macau</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1588</t>
+          <t>1642</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1588</t>
+          <t>1645</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Gonçalo Álvares</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Superior das residências de Kienning fou etc</t>
+          <t>Visitador das Índias e do Japão</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1567</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1567</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>José Montanha</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Superior das seis residências do Norte</t>
+          <t>Procurador</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1641</t>
+          <t>1753</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1650</t>
+          <t>1753</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Francisco Pérez</t>
+          <t>José Montanha</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Superior das Índias</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1552</t>
+          <t>1749</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1552</t>
+          <t>1752</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>João da Rocha</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Superior de Agra</t>
+          <t>Superior da missão da China</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1624</t>
+          <t>1622</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1624</t>
+          <t>1622</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Francisco Pérez</t>
+          <t>Leonardo Teixeira</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Superior de Macau</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1565</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1565</t>
+          <t>1699</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cristóvão da Costa</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Superior de Macau</t>
+          <t>Analista das missões da China e do Japão</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1576</t>
+          <t>1583</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1576</t>
+          <t>1596</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Monitor de Alessandro Valignano</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1579</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1654</t>
+          <t>1579</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Superior da residência de Macau</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1657</t>
+          <t>1588</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1659</t>
+          <t>1588</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1546,72 +1546,72 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1663</t>
+          <t>1623</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1654</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>António de Gouveia</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Visitador das missões</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1669</t>
+          <t>1614</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1672</t>
+          <t>1615</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Tomé (Sancho) Pereira</t>
+          <t>Manuel Gaspar</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Procurador da China e do Japão</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1692</t>
+          <t>1603</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1695</t>
+          <t>1603</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>António da Silva</t>
+          <t>Manuel Mendes</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1621,243 +1621,243 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1711</t>
+          <t>1714</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Manuel Mendes</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Procurador da Província do Japão em Macau</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>1705</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1705</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>António Gomes</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Reitor do colégio de Macau</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1748</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1751</t>
+          <t>1704</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Vice-provincial da China do Norte</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1635</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1641</t>
+          <t>1705</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>Manuel de Sá</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Vice-provincial da China do Sul</t>
+          <t>Socius de Francesco Maria Spinola</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1646</t>
+          <t>1694</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1646</t>
+          <t>1694</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Belchior Nunes Barreto</t>
+          <t>Mateus de Couros</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Vice-provincial das Índias Orientais</t>
+          <t>Provincial do Japão e da China</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1553</t>
+          <t>1617</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1553</t>
+          <t>1632</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Vice-provincial das Índias Orientais</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1556</t>
+          <t>1658</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1556</t>
+          <t>1661</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Belchior Nunes Barreto</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vice-provincial de Cochim</t>
+          <t>Reitor do Colégio de Macau</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1565</t>
+          <t>1666</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1565</t>
+          <t>1666</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1642</t>
+          <t>1663</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1645</t>
+          <t>1666</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Vice-reitor do Colégio de Macau</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1651</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1651</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1866,467 +1866,467 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1719</t>
+          <t>1694</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>1702</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1718</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Vice-reitor do Colégio de Macau</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>1719</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>1720</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Vice-visitador do Japão</t>
+          <t>Visitador da província de Goa</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1709</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Tomé (Sancho) Pereira</t>
+          <t>Nicolau Pimenta</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Vice-visitador do Japão e da China</t>
+          <t>Visitador das Índias Orientais</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1691</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1695</t>
+          <t>1613</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Belchior Nunes Barreto</t>
+          <t>Pedro Martins</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Visitador</t>
+          <t>Provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1566</t>
+          <t>1586</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1566</t>
+          <t>1586</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>António de Gouveia</t>
+          <t>Pedro Martins</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Visitador</t>
+          <t>Reitor de Goa</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1586</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1586</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Visitador da província de Goa</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1646</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1709</t>
+          <t>1649</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Visitador das missões</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1614</t>
+          <t>1650</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1615</t>
+          <t>1658</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>André Palmeiro</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Visitador das províncias de Goa e do Malabar</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1621</t>
+          <t>1648</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1626</t>
+          <t>1658</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>André Palmeiro</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Visitador das províncias do Malabar</t>
+          <t>Superior das residências de Kienning fou etc</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1618</t>
+          <t>1648</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1621</t>
+          <t>1648</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Nicolau Pimenta</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Visitador das Índias Orientais</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1595</t>
+          <t>1657</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>1659</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Gonçalo Álvares</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Visitador das Índias e do Japão</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1567</t>
+          <t>1659</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1567</t>
+          <t>1660</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Visitador de Agra</t>
+          <t>Provincial da Etiópia</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1624</t>
+          <t>1555</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1624</t>
+          <t>1555</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1559</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1572</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>André Palmeiro</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Superior da China</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1626</t>
+          <t>1559</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1635</t>
+          <t>1572</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Vice-provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1634</t>
+          <t>1556</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1634</t>
+          <t>1556</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Tomé (Sancho) Pereira</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1650</t>
+          <t>1692</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1695</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Tomé (Sancho) Pereira</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Vice-visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1659</t>
+          <t>1691</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1660</t>
+          <t>1695</t>
         </is>
       </c>
     </row>

</xml_diff>